<commit_message>
Add regression MATLAB notebook and update some data
</commit_message>
<xml_diff>
--- a/Experimental data/Yeast osmotic stress/Cytoplasmic RNA/Regression_exp1_CY5_cyt.xlsx
+++ b/Experimental data/Yeast osmotic stress/Cytoplasmic RNA/Regression_exp1_CY5_cyt.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s2342847_ed_ac_uk/Documents/Indistinguishability N gene-states Project/Figures for Paper/Figure 5 - Application to experimental data/Yeast, Osmotic shock response, RNA/Regression Results/Cytoplasmic RNA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\andrew\Projects\PowerLaw\Experimental data\Yeast osmotic stress\Cytoplasmic RNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{279B78CB-B1A5-4EE7-B844-AE35E176A59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3678D852-80C1-4E02-AC86-0B739C0CECED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77F50F-50CD-4FC7-9B92-C97C61E6D076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9FB31BCF-51E4-43B9-8F2F-5D14F31EBB18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{9FB31BCF-51E4-43B9-8F2F-5D14F31EBB18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -99,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +109,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,10 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,29 +466,29 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -494,7 +499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -532,24 +537,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>1.9170984455958599E-2</v>
+        <v>0.57098445595854896</v>
       </c>
       <c r="C4">
         <v>1930</v>
       </c>
       <c r="D4">
-        <v>1.8737672583826401E-2</v>
+        <v>0.57051282051282004</v>
       </c>
       <c r="E4">
         <v>2028</v>
       </c>
       <c r="F4" s="2">
-        <v>1.8948964123294599E-2</v>
+        <f>((B4*C4)+(D4*E4))/(G4)</f>
+        <v>0.57074279939363282</v>
       </c>
       <c r="G4">
         <f>C4+E4</f>
@@ -571,27 +577,28 @@
         <v>0.10749</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>2.6525198938992002E-3</v>
+        <v>0.44208664898319999</v>
       </c>
       <c r="C5">
         <v>1131</v>
       </c>
       <c r="D5">
-        <v>4.6168051708217897E-3</v>
+        <v>0.32317636195752503</v>
       </c>
       <c r="E5">
         <v>1083</v>
       </c>
       <c r="F5" s="2">
-        <v>3.613369467028E-3</v>
+        <f t="shared" ref="F5:F19" si="0">((B5*C5)+(D5*E5))/(G5)</f>
+        <v>0.38392050587172488</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G19" si="0">C5+E5</f>
+        <f t="shared" ref="G5:G19" si="1">C5+E5</f>
         <v>2214</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -610,51 +617,53 @@
         <v>6.1775999999999999E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="C6">
         <v>750</v>
       </c>
       <c r="D6">
-        <v>4.2573320719016101E-2</v>
+        <v>0.37842951750236498</v>
       </c>
       <c r="E6">
         <v>1057</v>
       </c>
       <c r="F6" s="2">
-        <v>2.4903154399557301E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.38904261206419466</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1807</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>5.0200803212851397E-3</v>
+        <v>0.83835341365461802</v>
       </c>
       <c r="C7">
         <v>996</v>
       </c>
       <c r="D7">
-        <v>0.126293995859213</v>
+        <v>1.1004140786749399</v>
       </c>
       <c r="E7">
         <v>966</v>
       </c>
       <c r="F7" s="2">
-        <v>6.4729867482161099E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.96738022426095394</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1962</v>
       </c>
       <c r="I7" t="s">
@@ -670,27 +679,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2.3230148048452199</v>
+        <v>3.7119784656796702</v>
       </c>
       <c r="C8">
         <v>743</v>
       </c>
       <c r="D8">
-        <v>2.3280542986425301</v>
+        <v>6.7330316742081404</v>
       </c>
       <c r="E8">
         <v>884</v>
       </c>
       <c r="F8" s="2">
-        <v>2.3257529194837101</v>
+        <f t="shared" si="0"/>
+        <v>5.3534111862323241</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1627</v>
       </c>
       <c r="I8">
@@ -706,277 +716,288 @@
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>13.5128</v>
+        <v>18.023199999999999</v>
       </c>
       <c r="C9">
         <v>1250</v>
       </c>
       <c r="D9">
-        <v>8.1951710261569399</v>
+        <v>16.486921529175</v>
       </c>
       <c r="E9">
         <v>497</v>
       </c>
       <c r="F9" s="2">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>17.586147681740112</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1747</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>20.8062730627306</v>
       </c>
       <c r="C10">
         <v>542</v>
       </c>
       <c r="D10">
-        <v>18.290730337078699</v>
+        <v>21.693820224719101</v>
       </c>
       <c r="E10">
         <v>712</v>
       </c>
-      <c r="F10">
-        <v>19.461722488038301</v>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>21.310207336523113</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1254</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>15.804136253041399</v>
+        <v>18.563260340632599</v>
       </c>
       <c r="C11">
         <v>822</v>
       </c>
       <c r="D11">
-        <v>19.398260869565199</v>
+        <v>24.756521739130399</v>
       </c>
       <c r="E11">
         <v>575</v>
       </c>
-      <c r="F11">
-        <v>17.283464566929101</v>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>21.112383679312799</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1397</v>
       </c>
       <c r="I11" s="1">
         <v>1160</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>7.6330434782608698</v>
+        <v>20.933043478260799</v>
       </c>
       <c r="C12">
         <v>1150</v>
       </c>
       <c r="D12">
-        <v>7.1752988047808799</v>
+        <v>26.806772908366501</v>
       </c>
       <c r="E12">
         <v>1004</v>
       </c>
-      <c r="F12">
-        <v>7.4196843082637001</v>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>23.670844939647115</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2154</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13">
-        <v>1.3417935702199699</v>
+        <v>14.3536379018612</v>
       </c>
       <c r="C13">
         <v>591</v>
       </c>
       <c r="D13">
-        <v>1.19463087248322</v>
+        <v>13.261744966442899</v>
       </c>
       <c r="E13">
         <v>149</v>
       </c>
-      <c r="F13">
-        <v>1.31216216216216</v>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>14.133783783783732</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>740</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>30</v>
       </c>
       <c r="B14">
-        <v>0.27283800243605399</v>
+        <v>13.57856272838</v>
       </c>
       <c r="C14">
         <v>821</v>
       </c>
       <c r="D14">
-        <v>0.29385964912280699</v>
+        <v>12.3815789473684</v>
       </c>
       <c r="E14">
         <v>228</v>
       </c>
-      <c r="F14">
-        <v>0.27740705433746399</v>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>13.318398474737821</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1049</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>35</v>
       </c>
       <c r="B15">
-        <v>2.8571428571428598E-2</v>
+        <v>6.9922077922077897</v>
       </c>
       <c r="C15">
         <v>385</v>
       </c>
       <c r="D15">
-        <v>8.1441922563417896E-2</v>
+        <v>8.4619492656875792</v>
       </c>
       <c r="E15">
         <v>749</v>
       </c>
-      <c r="F15">
-        <v>6.3492063492063502E-2</v>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>7.9629629629629601</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1134</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>40</v>
       </c>
       <c r="B16">
-        <v>6.1959654178674398E-2</v>
+        <v>6.8112391930835701</v>
       </c>
       <c r="C16">
         <v>694</v>
       </c>
       <c r="D16">
-        <v>1.9148936170212801E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E16">
         <v>470</v>
       </c>
-      <c r="F16">
-        <v>4.4673539518900303E-2</v>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8780068728522314</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1164</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>45</v>
       </c>
       <c r="B17">
-        <v>2.1912350597609601E-2</v>
+        <v>6.75</v>
       </c>
       <c r="C17">
         <v>1004</v>
       </c>
       <c r="D17">
-        <v>1.16279069767442E-2</v>
+        <v>4.8313953488371997</v>
       </c>
       <c r="E17">
         <v>344</v>
       </c>
-      <c r="F17">
-        <v>1.9287833827893199E-2</v>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>6.2603857566765555</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1348</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>50</v>
       </c>
       <c r="B18">
-        <v>2.6607538802660799E-2</v>
+        <v>6.9223946784922399</v>
       </c>
       <c r="C18">
         <v>451</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>4.2976190476190403</v>
       </c>
       <c r="E18">
         <v>84</v>
       </c>
-      <c r="F18">
-        <v>2.2429906542056101E-2</v>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>6.5102803738317752</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>535</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>55</v>
       </c>
       <c r="B19">
-        <v>1.7825311942958999E-2</v>
+        <v>8.8074866310160402</v>
       </c>
       <c r="C19">
         <v>1122</v>
       </c>
       <c r="D19">
-        <v>2.27272727272727E-2</v>
+        <v>7.9772727272727204</v>
       </c>
       <c r="E19">
         <v>528</v>
       </c>
-      <c r="F19">
-        <v>1.9393939393939401E-2</v>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5418181818181775</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1650</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
         <v>15</v>
       </c>

</xml_diff>